<commit_message>
Billing api service layer is connected to backend
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB79A2F-B455-C24B-9684-245642880957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A808EC-E9C0-CE4B-A672-8551A68CD065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="4660" windowWidth="25640" windowHeight="13360" xr2:uid="{15833022-3FF4-B545-AA8F-5A9E33D8B1E8}"/>
+    <workbookView xWindow="-10960" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{15833022-3FF4-B545-AA8F-5A9E33D8B1E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Ensure that the frontend can successfully retrieve and display data from the backend services</t>
   </si>
@@ -68,7 +68,13 @@
     <t>7. Teachers can delete subscriptions</t>
   </si>
   <si>
-    <t>Create billingSlice.js</t>
+    <t>Action: Create billingSlice.js</t>
+  </si>
+  <si>
+    <t>Action: map existing users in Admin service to Stripe Customer objects</t>
+  </si>
+  <si>
+    <t>Action: Generate a new customer when a user sets up billing for a student</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99150195-5828-9F48-9085-3B4E4693038E}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,36 +505,62 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="19" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="20" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="21" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update naming convention for BillingService thunks
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A808EC-E9C0-CE4B-A672-8551A68CD065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FA1113-3D14-024E-A74B-C196350D725F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10960" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{15833022-3FF4-B545-AA8F-5A9E33D8B1E8}"/>
+    <workbookView xWindow="-10960" yWindow="-28300" windowWidth="51200" windowHeight="27160" xr2:uid="{15833022-3FF4-B545-AA8F-5A9E33D8B1E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Ensure that the frontend can successfully retrieve and display data from the backend services</t>
   </si>
@@ -56,9 +56,6 @@
     <t>3. Teachers Can Create Customer</t>
   </si>
   <si>
-    <t>4. Teachers can Create Subscription for student</t>
-  </si>
-  <si>
     <t>5. Teachers can get billing history for students</t>
   </si>
   <si>
@@ -74,7 +71,16 @@
     <t>Action: map existing users in Admin service to Stripe Customer objects</t>
   </si>
   <si>
-    <t>Action: Generate a new customer when a user sets up billing for a student</t>
+    <t>requirements:</t>
+  </si>
+  <si>
+    <t>If no Stripe Customer entity exists for user, render a button to sign user up.</t>
+  </si>
+  <si>
+    <t>Component with form to sign user up for a billing Subscription (create Subscription)</t>
+  </si>
+  <si>
+    <t>Link existing ManageBilling Component to relevant dispatches</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99150195-5828-9F48-9085-3B4E4693038E}">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +508,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
@@ -512,7 +518,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -527,40 +533,71 @@
       </c>
     </row>
     <row r="15" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User feedback in billing components, and updates to redux state structure
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC0B2A-1D8A-1B49-BBD0-E1E259338CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-4420" yWindow="-24160" windowWidth="29860" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="New Components" sheetId="2" r:id="rId2"/>
+    <sheet name="General" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Release 0.3.0: Connect Frontend Billing components to Backend</t>
   </si>
@@ -59,14 +67,109 @@
   </si>
   <si>
     <t>7. Teachers can delete subscriptions</t>
+  </si>
+  <si>
+    <t>CreateStripeCustomer</t>
+  </si>
+  <si>
+    <t>Create Subscription</t>
+  </si>
+  <si>
+    <t>Component Should give feedback when customer is created</t>
+  </si>
+  <si>
+    <t>component should redirect back to student</t>
+  </si>
+  <si>
+    <t>Redux State should reset</t>
+  </si>
+  <si>
+    <t>Component Should give feedback when subscription is created</t>
+  </si>
+  <si>
+    <t>component should redirect back to student on success</t>
+  </si>
+  <si>
+    <t>Create Payment Method</t>
+  </si>
+  <si>
+    <t>Component should give feedback when payment method is created / confirmed</t>
+  </si>
+  <si>
+    <t>CreateSubscription component should fetch and render new payment methods in form when a new payment method is created</t>
+  </si>
+  <si>
+    <t>Component should fetch user by system id (useParams to get id in url)  if state is empty</t>
+  </si>
+  <si>
+    <t>Component should fetch Stripe customer (useParams to get id in url) if state is empty</t>
+  </si>
+  <si>
+    <t>General Issues/Enhancements</t>
+  </si>
+  <si>
+    <t>Refactor new components to use entity adapters instead of creating redundant state objects</t>
+  </si>
+  <si>
+    <t>Refactor remaining Redux reducers to use the entity namespaces</t>
+  </si>
+  <si>
+    <t>Remove poorly designed/unused backend classes</t>
+  </si>
+  <si>
+    <t>Refactor to PaymentElement instead of CardElement for creating payment methods</t>
+  </si>
+  <si>
+    <t>clearAll in billing when SingleStudent Component closes</t>
+  </si>
+  <si>
+    <t>Form Validation - disable submit button if formstate not complete</t>
+  </si>
+  <si>
+    <t>Issue: payment method not attaching to customer on creation</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Defect causing CreatePaymentMethod component to unmount on submitting form. Needs new solution</t>
+  </si>
+  <si>
+    <t>component should redirect back to CreateSubscription on success</t>
+  </si>
+  <si>
+    <t>Standalone version of New{PaymentMethod</t>
+  </si>
+  <si>
+    <t>Billing Overview</t>
+  </si>
+  <si>
+    <t>Button should render correctly when new customer is created</t>
+  </si>
+  <si>
+    <t>issue: race condition between creating customer within Stripe and re-rendering the billing overview component with correct condition.
+Fix: fetch stripeCustomerId directly from redux instead of the stripeCustomerId state property 
+Possible enhancement: CreateCustomer could be a child of CreateSubscription</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>resolution: conditional rendering caused paymentmethod modal to unmount on submit. Removed loadning state, but need to refactor use of loading state prop</t>
+  </si>
+  <si>
+    <t>issue: ccaused by similar race condition with creating customer in Stripe API and rendering billingOverview.
+Possible Solution: push id to redux and use that instead of fetching</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +196,33 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -121,32 +244,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -157,10 +286,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -198,71 +327,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -290,7 +419,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -313,11 +442,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -326,13 +455,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -342,7 +471,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -351,7 +480,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,7 +489,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -368,10 +497,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -436,170 +565,343 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+    <row r="8" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+    <row r="11" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+    <row r="12" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+    <row r="13" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row r="16" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row r="17" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
+    <row r="18" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+    <row r="19" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
+    <row r="20" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
+    <row r="22" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row r="23" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
-      <c r="A25" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
-      <c r="A26" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
-      <c r="A27" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
-      <c r="A28" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17">
-      <c r="A29" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17">
-      <c r="A30" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17">
-      <c r="A31" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17">
-      <c r="A32" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17">
-      <c r="A33" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
-      <c r="A34" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
-      <c r="A35" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
-      <c r="A36" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row r="25" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row r="38" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row r="39" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A75D66E-A352-F144-BAC5-E0F0591C330F}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="97.5" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="112" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEA0BDF-647C-5649-BAAD-28BBFED53411}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="68.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle resetting state on biliing component close and form validation
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC0B2A-1D8A-1B49-BBD0-E1E259338CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE19E78-D441-CC4E-A56A-4E7654C558AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4420" yWindow="-24160" windowWidth="29860" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Release 0.3.0: Connect Frontend Billing components to Backend</t>
   </si>
@@ -135,12 +135,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>Defect causing CreatePaymentMethod component to unmount on submitting form. Needs new solution</t>
-  </si>
-  <si>
-    <t>component should redirect back to CreateSubscription on success</t>
-  </si>
-  <si>
     <t>Standalone version of New{PaymentMethod</t>
   </si>
   <si>
@@ -150,19 +144,10 @@
     <t>Button should render correctly when new customer is created</t>
   </si>
   <si>
-    <t>issue: race condition between creating customer within Stripe and re-rendering the billing overview component with correct condition.
-Fix: fetch stripeCustomerId directly from redux instead of the stripeCustomerId state property 
-Possible enhancement: CreateCustomer could be a child of CreateSubscription</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
     <t>resolution: conditional rendering caused paymentmethod modal to unmount on submit. Removed loadning state, but need to refactor use of loading state prop</t>
-  </si>
-  <si>
-    <t>issue: ccaused by similar race condition with creating customer in Stripe API and rendering billingOverview.
-Possible Solution: push id to redux and use that instead of fetching</t>
   </si>
 </sst>
 </file>
@@ -205,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,12 +200,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -257,7 +236,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -710,39 +688,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A75D66E-A352-F144-BAC5-E0F0591C330F}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="97.5" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>45</v>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -750,12 +728,12 @@
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -773,27 +751,27 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -802,45 +780,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>37</v>
+      <c r="B16" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>38</v>
+      <c r="A18" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="112" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>42</v>
+      <c r="B22" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +827,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -868,7 +841,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -877,7 +850,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -887,7 +860,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -901,7 +874,7 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update reduxUtil to use entity adapter for more methods. Manage Subscriptions fetches subscription object
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE19E78-D441-CC4E-A56A-4E7654C558AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7C768B-5EB3-7546-87D2-21D38FE80F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4420" yWindow="-24160" windowWidth="29860" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="-14520" windowWidth="29860" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="New Components" sheetId="2" r:id="rId2"/>
     <sheet name="General" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Release 0.3.0: Connect Frontend Billing components to Backend</t>
   </si>
@@ -148,6 +161,12 @@
   </si>
   <si>
     <t>resolution: conditional rendering caused paymentmethod modal to unmount on submit. Removed loadning state, but need to refactor use of loading state prop</t>
+  </si>
+  <si>
+    <t>handle loading state</t>
+  </si>
+  <si>
+    <t>future enhancement</t>
   </si>
 </sst>
 </file>
@@ -223,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -240,6 +259,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -688,10 +711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A75D66E-A352-F144-BAC5-E0F0591C330F}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -738,82 +761,103 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="17" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -827,7 +871,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -848,6 +892,9 @@
       <c r="A2" t="s">
         <v>31</v>
       </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -855,7 +902,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -865,7 +912,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented service layer methods for Stripe meter and invoice CRUD
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7C768B-5EB3-7546-87D2-21D38FE80F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB029E92-0DE0-284A-9CE0-2DFDAE5FCEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="-14520" windowWidth="29860" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="New Components" sheetId="2" r:id="rId2"/>
     <sheet name="General" sheetId="3" r:id="rId3"/>
+    <sheet name="Final Release Features " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Release 0.3.0: Connect Frontend Billing components to Backend</t>
   </si>
@@ -167,6 +168,39 @@
   </si>
   <si>
     <t>future enhancement</t>
+  </si>
+  <si>
+    <t>Remaining Features:</t>
+  </si>
+  <si>
+    <t>Implement Invoices</t>
+  </si>
+  <si>
+    <t>Lesson Events should increment a Meter (Integrate event service)</t>
+  </si>
+  <si>
+    <t>Aattach Payment Methods to Subscriptions</t>
+  </si>
+  <si>
+    <t>Comments:</t>
+  </si>
+  <si>
+    <t>Subscriptions should genertate a monthly invoice</t>
+  </si>
+  <si>
+    <t>New API endpoints needed</t>
+  </si>
+  <si>
+    <t>Finish frontend ManagePaymentMethod component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesson Events should increment a Meter </t>
+  </si>
+  <si>
+    <t>Integrate event service</t>
+  </si>
+  <si>
+    <t>Setup Intents should get confirmed once created</t>
   </si>
 </sst>
 </file>
@@ -242,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -261,10 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A75D66E-A352-F144-BAC5-E0F0591C330F}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -803,11 +834,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="9"/>
     </row>
     <row r="17" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -868,10 +898,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEA0BDF-647C-5649-BAAD-28BBFED53411}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A9" sqref="A9:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -889,39 +919,124 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
+      <c r="A2" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B6" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF78B9-DDE0-414B-8D96-26D041FC07FC}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="68.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created LogLesson component for creating Lesson MeterEvents
</commit_message>
<xml_diff>
--- a/turbolessons-frontend/spec/Billing Release.xlsx
+++ b/turbolessons-frontend/spec/Billing Release.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noslen/DevProjects/TurboLessons_Frontend/turbolessons-frontend/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94212CD-264A-F34F-964A-72595E7E5602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C114E93-4009-5849-9E24-18F73CA00D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7420" yWindow="-23380" windowWidth="28800" windowHeight="15300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="New Components" sheetId="2" r:id="rId2"/>
     <sheet name="General" sheetId="3" r:id="rId3"/>
     <sheet name="Final Release Features " sheetId="4" r:id="rId4"/>
+    <sheet name="Invoice Feature" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>Release 0.3.0: Connect Frontend Billing components to Backend</t>
   </si>
@@ -216,6 +217,43 @@
   </si>
   <si>
     <t>Finish ManageSubscription.jsx Subscription Details</t>
+  </si>
+  <si>
+    <t>Use Case: User has no payment method set up</t>
+  </si>
+  <si>
+    <t>find pm for customer if one exists, otherwise create pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update request using pm for that </t>
+  </si>
+  <si>
+    <t>Feature Objectives:</t>
+  </si>
+  <si>
+    <t>Steps to implement:</t>
+  </si>
+  <si>
+    <t>Create a workflow for marking lesson attendance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Render new component within:
+/src/pages/Teachers/Lessons.jsx
+</t>
+  </si>
+  <si>
+    <t>components:
+LessonList - show all lessons for teacher in the month</t>
+  </si>
+  <si>
+    <t>when a lesson event is logged, dispatch API Call to create a corresponding MeterEvent object</t>
+  </si>
+  <si>
+    <t>Within LessonList table - Render Button for 'Mark Attendance' 
+(Only Enable if current date &gt; lessonDate)</t>
+  </si>
+  <si>
+    <t>Email/Message service should send a system message reminding teachers to log lessons before invoices are finalized</t>
   </si>
 </sst>
 </file>
@@ -617,7 +655,7 @@
   </sheetPr>
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -995,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDF78B9-DDE0-414B-8D96-26D041FC07FC}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1040,19 +1078,11 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1073,6 +1103,99 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B16EAB0-CAF9-5E41-B3DA-7361FDE17C2C}">
+  <dimension ref="B1:C9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="C8" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>